<commit_message>
Add another case in xlsx file
</commit_message>
<xml_diff>
--- a/TestCase5.xlsx
+++ b/TestCase5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IMPERIUMOFRACOONKIND\Desktop\Программирование\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IMPERIUMOFRACOONKIND\Desktop\Программирование\GitHub\TestCases\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CEB3338-DF73-4E09-91F2-A106D93CA4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EED827F-318C-473D-829C-26F84A03FFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>1.0</t>
   </si>
@@ -80,16 +80,7 @@
     <t>Результат</t>
   </si>
   <si>
-    <t>Товар, отсутствующий в продаже попадает в корзину</t>
-  </si>
-  <si>
     <t>Отображение товара, отсутствующего в продаже</t>
-  </si>
-  <si>
-    <t>Товар, отсутствующий в продаже нельзя положить в  корзину</t>
-  </si>
-  <si>
-    <t>Товар, отсутствующий в продаже возможно положить в  корзину</t>
   </si>
   <si>
     <t>Предусловия</t>
@@ -108,6 +99,29 @@
 4. Зайти в корзину
 5. Нажать "Оформить заказ"
 </t>
+  </si>
+  <si>
+    <t>Откроется страница с оплатой заказа.</t>
+  </si>
+  <si>
+    <t>Появляется сообщение о том, что товар отсутствует.</t>
+  </si>
+  <si>
+    <t>Оформление заказа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Зайти в Каталог
+2. Выбрать "Мясо и птица"
+</t>
+  </si>
+  <si>
+    <t>Товар "Крылья куриные охлажденные" недоступен для добавления в корзину, поскольку отсутствует в наличии</t>
+  </si>
+  <si>
+    <t>Товар "Крылья куриные охлажденные" добавляется в корзину, сообщение об отсутствии товара появляется не при попытке добавить товар в корзину, а при оформлении заказа и готовности его оплатить.</t>
+  </si>
+  <si>
+    <t>Товар, отсутствующий в продажу добавляется в корзину</t>
   </si>
 </sst>
 </file>
@@ -192,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -449,11 +463,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -470,112 +588,148 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -867,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,76 +1037,80 @@
     <col min="6" max="6" width="11.21875" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" customWidth="1"/>
+    <col min="9" max="9" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="7">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="12">
         <v>45477</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="6" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
     </row>
-    <row r="4" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="6" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="41"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="52"/>
     </row>
-    <row r="5" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="6" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="41"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="53"/>
     </row>
-    <row r="6" spans="1:7" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:9" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -961,95 +1119,115 @@
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>21</v>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="39"/>
+      <c r="H6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="24"/>
-    </row>
-    <row r="7" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>22</v>
+      <c r="D7" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="26"/>
+      <c r="F7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="40"/>
+      <c r="H7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:7" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="18"/>
+    <row r="8" spans="1:9" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="37"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="28"/>
+      <c r="F8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="41"/>
+      <c r="H8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:7" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33" t="s">
+    <row r="9" spans="1:9" ht="120.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="38"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="35"/>
+      <c r="F9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="42"/>
+      <c r="H9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
+  <mergeCells count="22">
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="D7:D9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>